<commit_message>
Reclassifies camp scrimmage as scrimmage.
</commit_message>
<xml_diff>
--- a/event_type.xlsx
+++ b/event_type.xlsx
@@ -31,13 +31,13 @@
     <t>camp</t>
   </si>
   <si>
+    <t>scrimmage</t>
+  </si>
+  <si>
     <t>tues</t>
   </si>
   <si>
     <t>wed</t>
-  </si>
-  <si>
-    <t>scrimmage</t>
   </si>
   <si>
     <t>thurs</t>
@@ -153,14 +153,11 @@
   </sheetPr>
   <dimension ref="A1:B72"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B66" activeCellId="0" sqref="B66"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -247,7 +244,7 @@
         <v>42956</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -319,7 +316,7 @@
         <v>42967</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -327,7 +324,7 @@
         <v>42969</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -335,7 +332,7 @@
         <v>42970</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -343,7 +340,7 @@
         <v>42971</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -351,7 +348,7 @@
         <v>42972</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -359,7 +356,7 @@
         <v>42973</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -391,7 +388,7 @@
         <v>42983</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -399,7 +396,7 @@
         <v>42984</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -423,7 +420,7 @@
         <v>42990</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -431,7 +428,7 @@
         <v>42991</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -455,7 +452,7 @@
         <v>42997</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -463,7 +460,7 @@
         <v>42998</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -487,7 +484,7 @@
         <v>43004</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -495,7 +492,7 @@
         <v>43005</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -519,7 +516,7 @@
         <v>43011</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -551,7 +548,7 @@
         <v>43018</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -559,7 +556,7 @@
         <v>43019</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -583,7 +580,7 @@
         <v>43025</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -591,7 +588,7 @@
         <v>43026</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -615,7 +612,7 @@
         <v>43032</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -639,7 +636,7 @@
         <v>43039</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -671,7 +668,7 @@
         <v>43047</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -679,7 +676,7 @@
         <v>43048</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -711,7 +708,7 @@
         <v>43060</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -719,7 +716,7 @@
         <v>43061</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>